<commit_message>
Version V0.1 sended to fabrication
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -12,11 +12,13 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
-    <sheet name="Untitled" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Untitled" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="bom" localSheetId="0">Hoja1!$A$1:$H$22</definedName>
+    <definedName name="bom" localSheetId="1">Hoja1!$A$1:$H$21</definedName>
+    <definedName name="test" localSheetId="0">Hoja2!$A$1:$E$22</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -43,11 +45,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="test" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/darkomen/ESP12_pcb/test.csv" decimal="," thousands="." tab="0" delimiter=",">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="104">
   <si>
     <t>QTY,Refs,Value,Footprint,MFR,MPN,SPR,SPN</t>
   </si>
@@ -211,118 +224,154 @@
     <t>Diodes_SMD:D_SOD-123F</t>
   </si>
   <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN_01X02</t>
+  </si>
+  <si>
+    <t>Pin_Headers:Pin_Header_Straight_1x02_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>0603L100SLYR</t>
+  </si>
+  <si>
+    <t>Resistors_SMD:R_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>1,87M</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>2M</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>340k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>390k</t>
+  </si>
+  <si>
+    <t>Q2;Q1</t>
+  </si>
+  <si>
+    <t>IRLML9301TRPBF</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LD1117DT33TR</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:TO-252-2Lead</t>
+  </si>
+  <si>
+    <t>C1;C2</t>
+  </si>
+  <si>
+    <t>papayagroup:C_3528</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>6.8uH</t>
+  </si>
+  <si>
+    <t>papayagroup:L_bourns</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TPS61090</t>
+  </si>
+  <si>
+    <t>papayagroup:QFN65P400X400X100-17N</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>ZX62D1-B-5PA(30)</t>
+  </si>
+  <si>
+    <t>papayagroup:USB-micro-B_Hirose</t>
+  </si>
+  <si>
+    <t>datasheet</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/walsin/0603f104z250ct/condens-mlcc-y5v-0-1uf-25v-0603/dp/2496873</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/tdk/c1608x5r1a106k080ac/cond-cer-mult-x5r-10uf-10v-0603/dp/2211164</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/avx/06036c225kat2a/cond-cer-mult-x7r-2-2uf-6-3v-0603/dp/1657930</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/murata/grm21br60j107me15l/cond-mlcc-x5r-100uf-6-3v-0805/dp/2494476</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/on-semiconductor/mbr120vlsft3g/rectificador-schottky-1a-20v-sod123/dp/2533227</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
     <t>3V3;12V1;5V1;VDD1;LBO1;GND1</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>Measurement_Points:Measurement_Point_Round-SMD-Pad_Small</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>CONN_01X02</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x02_Pitch2.54mm</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>0603L100SLYR</t>
-  </si>
-  <si>
-    <t>Resistors_SMD:R_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>1,87M</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>200k</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>2M</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>340k</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>390k</t>
-  </si>
-  <si>
-    <t>Q2;Q1</t>
-  </si>
-  <si>
-    <t>IRLML9301TRPBF</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:SOT-23</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>LD1117DT33TR</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:TO-252-2Lead</t>
-  </si>
-  <si>
-    <t>C1;C2</t>
-  </si>
-  <si>
-    <t>papayagroup:C_3528</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>6.8uH</t>
-  </si>
-  <si>
-    <t>papayagroup:L_bourns</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TPS61090</t>
-  </si>
-  <si>
-    <t>papayagroup:QFN65P400X400X100-17N</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>ZX62D1-B-5PA(30)</t>
-  </si>
-  <si>
-    <t>papayagroup:USB-micro-B_Hirose</t>
+    <t>http://es.farnell.com/littelfuse/0603l100slyr/fuse-resettable-ptc-6vdc-1a-smd/dp/2545623?st=fuse+0603&amp;pf=510192206&amp;corriente-de-disparo=1.8a&amp;anyFilterApplied=true&amp;ddkey=http%3Aes-ES%2FElement14_Spain%2Fw%2Fc%2Fproteccion-de-circuitos%2Ftermistores%2Ffusibles-rearmables-pptc</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/infineon/irlml9301trpbf/mosfet-diode-p-ch-30v-3-6a-sot23/dp/1831089</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/stmicroelectronics/ld1117dt33tr/reg-tensi-n-ldo-3-3v-smd-1117/dp/1087169RL</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/avx/tajb106k016rnj/cond-tant-10uf-16v-encap-b/dp/498737</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/coiltronics/dr1030-6r8-r/inductor-blindado-6-8uh-3-5a/dp/2145105?ost=CDRH103RNP-6R8NC-B&amp;searchView=table&amp;iscrfnonsku=true&amp;ddkey=http%3Aes-ES%2FElement14_Spain%2Fsearch</t>
+  </si>
+  <si>
+    <t>http://es.farnell.com/texas-instruments/tps61090rsarg4/boost-converter-0-5a-adj-61090/dp/1207334</t>
   </si>
 </sst>
 </file>
@@ -375,6 +424,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bom" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -641,10 +694,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,7 +1190,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -808,7 +1227,7 @@
         <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -816,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -830,13 +1249,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -844,13 +1263,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -858,13 +1277,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -872,32 +1291,32 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
         <v>71</v>
       </c>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>75</v>
@@ -911,27 +1330,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>78</v>
       </c>
       <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
         <v>79</v>
-      </c>
-      <c r="D18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
         <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>82</v>
@@ -963,20 +1382,6 @@
       </c>
       <c r="D21" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>

</xml_diff>